<commit_message>
new scenario with random population
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C74693-E8FE-4993-B078-862BE46D515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA315356-4A13-4B98-96E8-B8836B0FF1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>case_x</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>population_per_cell</t>
+  </si>
+  <si>
+    <t>population_type</t>
+  </si>
+  <si>
+    <t>uniform</t>
+  </si>
+  <si>
+    <t>random</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,6 +648,50 @@
         <v>250</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>850</v>
+      </c>
+      <c r="C20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>650</v>
+      </c>
+      <c r="C21">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>450</v>
+      </c>
+      <c r="C22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>750</v>
+      </c>
+      <c r="C23">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -646,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,6 +844,34 @@
         <v>855</v>
       </c>
       <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>105</v>
+      </c>
+      <c r="C12">
+        <v>855</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -802,48 +883,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
best combination and chains to investigate
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA315356-4A13-4B98-96E8-B8836B0FF1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95671AFF-C5E5-4955-88A1-DE76F83BCC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="-25693" yWindow="-3907" windowWidth="25786" windowHeight="13867" activeTab="2" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>case_x</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t>Chain 2</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -92,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,6 +708,72 @@
         <v>250</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>150</v>
+      </c>
+      <c r="C24">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>250</v>
+      </c>
+      <c r="C25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>350</v>
+      </c>
+      <c r="C26">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>550</v>
+      </c>
+      <c r="C27">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>250</v>
+      </c>
+      <c r="C28">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>550</v>
+      </c>
+      <c r="C29">
+        <v>850</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -699,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,6 +955,174 @@
       </c>
       <c r="D12" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>115</v>
+      </c>
+      <c r="C13">
+        <v>825</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>230</v>
+      </c>
+      <c r="C14">
+        <v>735</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>345</v>
+      </c>
+      <c r="C15">
+        <v>855</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>820</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>235</v>
+      </c>
+      <c r="C17">
+        <v>730</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>340</v>
+      </c>
+      <c r="C18">
+        <v>850</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>230</v>
+      </c>
+      <c r="C19">
+        <v>735</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>223</v>
+      </c>
+      <c r="C20">
+        <v>245</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>523</v>
+      </c>
+      <c r="C21">
+        <v>822</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>546</v>
+      </c>
+      <c r="C22">
+        <v>555</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>233</v>
+      </c>
+      <c r="C23">
+        <v>735</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>524</v>
+      </c>
+      <c r="C24">
+        <v>829</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -883,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,7 +1146,7 @@
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -906,8 +1156,14 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -918,7 +1174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -929,7 +1185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -940,12 +1196,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new traceback model based on Diggle et al. (1997)
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra.Rudeloff\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE63967-13B6-4383-B004-F8DE374AA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F8AFE-7849-4D2A-B87F-390D5FCBD985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>case_x</t>
   </si>
@@ -476,18 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -498,9 +498,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>750</v>
@@ -509,9 +509,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>150</v>
@@ -520,29 +520,29 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="C4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>450</v>
-      </c>
-      <c r="C5">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -550,87 +550,87 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>850</v>
+        <v>450</v>
       </c>
       <c r="C7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>850</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>850</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="C9">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>850</v>
       </c>
       <c r="C10">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>950</v>
+      </c>
+      <c r="C11">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>750</v>
-      </c>
-      <c r="C11">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>50</v>
       </c>
       <c r="C12">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="C13">
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -638,164 +638,164 @@
         <v>50</v>
       </c>
       <c r="C14">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
         <v>150</v>
       </c>
-      <c r="C15">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>150</v>
+      </c>
+      <c r="C17">
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>850</v>
-      </c>
-      <c r="C16">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>650</v>
-      </c>
-      <c r="C17">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18">
-        <v>450</v>
+        <v>850</v>
       </c>
       <c r="C18">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19">
+        <v>650</v>
+      </c>
+      <c r="C19">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>450</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
         <v>750</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>850</v>
-      </c>
-      <c r="C20">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>650</v>
-      </c>
-      <c r="C21">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22">
-        <v>450</v>
+        <v>850</v>
       </c>
       <c r="C22">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23">
+        <v>650</v>
+      </c>
+      <c r="C23">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>450</v>
+      </c>
+      <c r="C24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
         <v>750</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>150</v>
-      </c>
-      <c r="C24">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>250</v>
-      </c>
-      <c r="C25">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="C26">
         <v>850</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>550</v>
+        <v>250</v>
       </c>
       <c r="C27">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="C28">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -803,32 +803,32 @@
         <v>550</v>
       </c>
       <c r="C29">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>250</v>
+      </c>
+      <c r="C30">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>550</v>
+      </c>
+      <c r="C31">
         <v>850</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>550</v>
-      </c>
-      <c r="C30">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31">
-        <v>250</v>
-      </c>
-      <c r="C31">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -836,32 +836,32 @@
         <v>550</v>
       </c>
       <c r="C32">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>250</v>
+      </c>
+      <c r="C33">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>550</v>
+      </c>
+      <c r="C34">
         <v>850</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>550</v>
-      </c>
-      <c r="C33">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>8</v>
-      </c>
-      <c r="B34">
-        <v>250</v>
-      </c>
-      <c r="C34">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>8</v>
       </c>
@@ -869,6 +869,28 @@
         <v>550</v>
       </c>
       <c r="C35">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>250</v>
+      </c>
+      <c r="C36">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>550</v>
+      </c>
+      <c r="C37">
         <v>850</v>
       </c>
     </row>
@@ -879,15 +901,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D48" sqref="A37:D48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -901,9 +923,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>112</v>
@@ -915,9 +937,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>823</v>
@@ -929,79 +951,79 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>823</v>
+      </c>
+      <c r="C5">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>888</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>846</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>105</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>855</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>487</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>537</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>2</v>
-      </c>
-      <c r="B7">
-        <v>112</v>
-      </c>
-      <c r="C7">
-        <v>198</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>105</v>
-      </c>
-      <c r="C8">
-        <v>855</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
       </c>
       <c r="B9">
         <v>112</v>
@@ -1013,9 +1035,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>105</v>
@@ -1027,9 +1049,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>112</v>
@@ -1041,9 +1063,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>105</v>
@@ -1055,339 +1077,367 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C13">
-        <v>825</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>230</v>
+        <v>105</v>
       </c>
       <c r="C14">
-        <v>735</v>
+        <v>855</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
       <c r="B15">
-        <v>345</v>
+        <v>115</v>
       </c>
       <c r="C15">
-        <v>855</v>
+        <v>825</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="C16">
-        <v>820</v>
+        <v>735</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17">
-        <v>235</v>
+        <v>345</v>
       </c>
       <c r="C17">
-        <v>730</v>
+        <v>855</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
-        <v>340</v>
+        <v>120</v>
       </c>
       <c r="C18">
-        <v>850</v>
+        <v>820</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
+        <v>235</v>
+      </c>
+      <c r="C19">
+        <v>730</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>340</v>
+      </c>
+      <c r="C20">
+        <v>850</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
         <v>230</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>735</v>
       </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
         <v>223</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>245</v>
       </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
         <v>523</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>822</v>
       </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
         <v>546</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>555</v>
       </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23">
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
         <v>233</v>
-      </c>
-      <c r="C23">
-        <v>735</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <v>524</v>
-      </c>
-      <c r="C24">
-        <v>829</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>230</v>
       </c>
       <c r="C25">
         <v>735</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>223</v>
+        <v>524</v>
       </c>
       <c r="C26">
-        <v>245</v>
+        <v>829</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
       <c r="B27">
-        <v>523</v>
+        <v>230</v>
       </c>
       <c r="C27">
-        <v>822</v>
+        <v>735</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
       <c r="B28">
-        <v>546</v>
+        <v>223</v>
       </c>
       <c r="C28">
-        <v>555</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
       <c r="B29">
-        <v>233</v>
+        <v>523</v>
       </c>
       <c r="C29">
-        <v>735</v>
+        <v>822</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
       <c r="B30">
-        <v>524</v>
+        <v>546</v>
       </c>
       <c r="C30">
-        <v>829</v>
+        <v>555</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C31">
         <v>735</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32">
-        <v>223</v>
+        <v>524</v>
       </c>
       <c r="C32">
-        <v>245</v>
+        <v>829</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
       <c r="B33">
-        <v>523</v>
+        <v>230</v>
       </c>
       <c r="C33">
-        <v>822</v>
+        <v>735</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8</v>
       </c>
       <c r="B34">
-        <v>546</v>
+        <v>223</v>
       </c>
       <c r="C34">
-        <v>555</v>
+        <v>245</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>8</v>
       </c>
       <c r="B35">
-        <v>750</v>
+        <v>523</v>
       </c>
       <c r="C35">
-        <v>735</v>
+        <v>822</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
       <c r="B36">
+        <v>546</v>
+      </c>
+      <c r="C36">
+        <v>555</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
         <v>750</v>
       </c>
-      <c r="C36">
+      <c r="C37">
+        <v>735</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>750</v>
+      </c>
+      <c r="C38">
         <v>829</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1399,22 +1449,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1444,9 +1494,9 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1457,9 +1507,9 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1470,12 +1520,12 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>500</v>
@@ -1483,12 +1533,12 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>500</v>
@@ -1496,9 +1546,9 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1509,26 +1559,22 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>500</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="1">
-        <v>50</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1537,15 +1583,15 @@
         <v>5000</v>
       </c>
       <c r="D9" s="1">
-        <v>5000</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1554,15 +1600,15 @@
         <v>5000</v>
       </c>
       <c r="D10" s="1">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="E10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1571,30 +1617,32 @@
         <v>5000</v>
       </c>
       <c r="D11" s="1">
-        <v>300</v>
+        <v>2500</v>
       </c>
       <c r="E11" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D12" s="1">
         <v>300</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1603,30 +1651,28 @@
         <v>10000</v>
       </c>
       <c r="D13" s="1">
+        <v>300</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D14" s="1">
         <v>1500</v>
       </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -1638,12 +1684,12 @@
         <v>100</v>
       </c>
       <c r="E15" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
@@ -1652,9 +1698,26 @@
         <v>5000</v>
       </c>
       <c r="D16" s="1">
+        <v>100</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D17" s="1">
         <v>1500</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scenario 1 was duplicate
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F8AFE-7849-4D2A-B87F-390D5FCBD985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904174EF-56B7-4DB2-B578-9C278DE99DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
   <si>
     <t>case_x</t>
   </si>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1449,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1522,10 +1522,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>500</v>
@@ -1535,10 +1535,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>500</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1561,20 +1561,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>5000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1583,7 +1587,7 @@
         <v>5000</v>
       </c>
       <c r="D9" s="1">
-        <v>50</v>
+        <v>5000</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1591,7 +1595,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1600,15 +1604,15 @@
         <v>5000</v>
       </c>
       <c r="D10" s="1">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1617,32 +1621,30 @@
         <v>5000</v>
       </c>
       <c r="D11" s="1">
-        <v>2500</v>
+        <v>300</v>
       </c>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="D12" s="1">
         <v>300</v>
       </c>
-      <c r="E12" s="1">
-        <v>4</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1651,28 +1653,30 @@
         <v>10000</v>
       </c>
       <c r="D13" s="1">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D14" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -1684,12 +1688,12 @@
         <v>100</v>
       </c>
       <c r="E15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
@@ -1698,26 +1702,9 @@
         <v>5000</v>
       </c>
       <c r="D16" s="1">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="E16" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E17" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lower bounds for parameters
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904174EF-56B7-4DB2-B578-9C278DE99DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288A50B8-20AD-48EA-9531-3735B781FD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>case_x</t>
   </si>
@@ -130,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,15 +153,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,11 +488,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -894,6 +904,17 @@
         <v>850</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>650</v>
+      </c>
+      <c r="C38">
+        <v>750</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -901,11 +922,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1439,6 +1458,20 @@
       </c>
       <c r="D38" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>550</v>
+      </c>
+      <c r="C39">
+        <v>550</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1449,11 +1482,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1708,6 +1739,19 @@
         <v>2</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>500</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new setup for shops
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F82233-54ED-4CA3-AC46-F3EA5C89F896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A49C8-D0DD-493C-909E-6C5FD7A59DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
     <sheet name="Store_Locations" sheetId="2" r:id="rId2"/>
     <sheet name="Population" sheetId="3" r:id="rId3"/>
+    <sheet name="Stores" sheetId="4" r:id="rId4"/>
+    <sheet name="Chain_Details" sheetId="5" r:id="rId5"/>
+    <sheet name="Explanation of Options" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>case_x</t>
   </si>
@@ -49,9 +52,6 @@
     <t>chain</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
     <t>store_x</t>
   </si>
   <si>
@@ -86,13 +86,52 @@
   </si>
   <si>
     <t>linear</t>
+  </si>
+  <si>
+    <t>no_of_chains</t>
+  </si>
+  <si>
+    <t>scenario_id</t>
+  </si>
+  <si>
+    <t>chain_id</t>
+  </si>
+  <si>
+    <t>num_stores</t>
+  </si>
+  <si>
+    <t>spatial_distribution</t>
+  </si>
+  <si>
+    <t>sales_distribution</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>total_sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population </t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>total_population, desired_gradient</t>
+  </si>
+  <si>
+    <t>total_population, desired_gradient, num_clusters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +141,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -150,27 +197,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,9 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C9A12-737E-45B0-A329-7250B15CD6A3}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -498,7 +536,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -923,19 +961,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -952,7 +992,7 @@
         <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -966,7 +1006,7 @@
         <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +1020,7 @@
         <v>198</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -994,7 +1034,7 @@
         <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,7 +1048,7 @@
         <v>846</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1022,7 +1062,7 @@
         <v>855</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1036,7 +1076,7 @@
         <v>537</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1050,7 +1090,7 @@
         <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1064,7 +1104,7 @@
         <v>855</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1078,7 +1118,7 @@
         <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1092,7 +1132,7 @@
         <v>855</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1106,7 +1146,7 @@
         <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1120,7 +1160,7 @@
         <v>855</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1134,7 +1174,7 @@
         <v>825</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1148,7 +1188,7 @@
         <v>735</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1162,7 +1202,7 @@
         <v>855</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,7 +1216,7 @@
         <v>820</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1190,7 +1230,7 @@
         <v>730</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1204,7 +1244,7 @@
         <v>850</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1218,7 +1258,7 @@
         <v>735</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1232,7 +1272,7 @@
         <v>245</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1246,7 +1286,7 @@
         <v>822</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,7 +1300,7 @@
         <v>555</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1274,7 +1314,7 @@
         <v>735</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1288,7 +1328,7 @@
         <v>829</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1302,7 +1342,7 @@
         <v>735</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1316,7 +1356,7 @@
         <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1330,7 +1370,7 @@
         <v>822</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1344,7 +1384,7 @@
         <v>555</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1358,7 +1398,7 @@
         <v>735</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1372,7 +1412,7 @@
         <v>829</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1386,7 +1426,7 @@
         <v>735</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1400,7 +1440,7 @@
         <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1414,7 +1454,7 @@
         <v>822</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1428,7 +1468,7 @@
         <v>555</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1442,7 +1482,7 @@
         <v>735</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1456,7 +1496,7 @@
         <v>829</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1470,7 +1510,7 @@
         <v>550</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1484,13 +1524,13 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
@@ -1498,19 +1538,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1518,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>500</v>
@@ -1531,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>500</v>
@@ -1544,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
@@ -1557,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>500</v>
@@ -1570,7 +1610,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>500</v>
@@ -1583,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -1596,13 +1636,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>5000</v>
       </c>
       <c r="D8" s="1">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1613,13 +1653,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>5000</v>
       </c>
       <c r="D9" s="1">
-        <v>5000</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1630,13 +1670,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>5000</v>
       </c>
       <c r="D10" s="1">
-        <v>2500</v>
+        <v>2.5</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
@@ -1647,13 +1687,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <v>5000</v>
       </c>
       <c r="D11" s="1">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -1664,13 +1704,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>10000</v>
       </c>
       <c r="D12" s="1">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1679,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>10000</v>
       </c>
       <c r="D13" s="1">
-        <v>1500</v>
+        <v>1.5</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1694,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>5000</v>
       </c>
       <c r="D14" s="1">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="E14" s="1">
         <v>5</v>
@@ -1711,13 +1751,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D15" s="1">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1728,24 +1768,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
         <v>5000</v>
       </c>
       <c r="D16" s="1">
-        <v>1500</v>
+        <v>1.5</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1">
         <v>500</v>
@@ -1756,4 +1796,216 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBD4BC-2492-48FA-B5D4-9D55D67013E4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68C25E-78FC-45FA-8783-AFBB87773DC1}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4211E5B7-A40C-4F39-A0BD-B28B4E6A2487}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NOT A WORKING VERSION - tried implementation w/ outbreak generation
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/scenarios.xlsx
+++ b/Traceback_Model/Data/scenarios.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra.Rudeloff\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A49C8-D0DD-493C-909E-6C5FD7A59DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6B891-C291-4EFC-9180-6ABF932403BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26397D4F-F0AB-4736-9A81-1ABFC6D3FF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbreak_Locations" sheetId="1" r:id="rId1"/>
-    <sheet name="Store_Locations" sheetId="2" r:id="rId2"/>
-    <sheet name="Population" sheetId="3" r:id="rId3"/>
-    <sheet name="Stores" sheetId="4" r:id="rId4"/>
-    <sheet name="Chain_Details" sheetId="5" r:id="rId5"/>
-    <sheet name="Explanation of Options" sheetId="6" r:id="rId6"/>
+    <sheet name="Outbreak" sheetId="7" r:id="rId2"/>
+    <sheet name="Store_Locations" sheetId="2" r:id="rId3"/>
+    <sheet name="Population" sheetId="3" r:id="rId4"/>
+    <sheet name="Stores" sheetId="4" r:id="rId5"/>
+    <sheet name="Chain_Details" sheetId="5" r:id="rId6"/>
+    <sheet name="Explanation of Options" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t>case_x</t>
   </si>
@@ -125,6 +126,12 @@
   </si>
   <si>
     <t>total_population, desired_gradient, num_clusters</t>
+  </si>
+  <si>
+    <t>list_outbreak_scenario_sizes</t>
+  </si>
+  <si>
+    <t>10, 20</t>
   </si>
 </sst>
 </file>
@@ -201,16 +208,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,12 +534,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -545,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -556,7 +561,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -567,7 +572,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -578,7 +583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -589,7 +594,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -600,7 +605,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -611,7 +616,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -622,7 +627,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -633,7 +638,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -644,7 +649,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -655,7 +660,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -666,7 +671,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -677,7 +682,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -688,7 +693,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -699,7 +704,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -710,7 +715,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -721,7 +726,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -732,7 +737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -743,7 +748,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -754,7 +759,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -765,7 +770,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -776,7 +781,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -787,7 +792,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -798,7 +803,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -809,7 +814,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -820,7 +825,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -831,7 +836,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
@@ -842,7 +847,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -853,7 +858,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -864,7 +869,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -875,7 +880,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -886,7 +891,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -897,7 +902,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -908,7 +913,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -919,7 +924,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
@@ -930,7 +935,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -941,7 +946,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -958,6 +963,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D2DD75-64B9-4611-81CD-049C64E4C3BB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E63A60-46A5-4F86-B9A0-EDE5315557A8}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -965,9 +1008,9 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -981,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -995,7 +1038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1009,7 +1052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1023,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1037,7 +1080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1051,7 +1094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1065,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1079,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1093,7 +1136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1107,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1121,7 +1164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1135,7 +1178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1149,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1163,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1177,7 +1220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1191,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1205,7 +1248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1219,7 +1262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1233,7 +1276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1247,7 +1290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1261,7 +1304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1275,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1289,7 +1332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1303,7 +1346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1317,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1331,7 +1374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1345,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1359,7 +1402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1373,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1387,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1401,7 +1444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1415,7 +1458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1429,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -1443,7 +1486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1457,7 +1500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
@@ -1471,7 +1514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -1485,7 +1528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8</v>
       </c>
@@ -1499,7 +1542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>16</v>
       </c>
@@ -1519,24 +1562,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FEEE3-41DA-4A9B-B6DA-1E3802A3E906}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1553,7 +1596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1566,7 +1609,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1579,7 +1622,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1592,7 +1635,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1605,7 +1648,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1618,7 +1661,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1631,7 +1674,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1648,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1665,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1682,7 +1725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1699,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1714,7 +1757,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1729,7 +1772,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1746,7 +1789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1763,7 +1806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1780,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1798,7 +1841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBD4BC-2492-48FA-B5D4-9D55D67013E4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1806,13 +1849,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1820,95 +1863,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68C25E-78FC-45FA-8783-AFBB87773DC1}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1917,26 +1877,109 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68C25E-78FC-45FA-8783-AFBB87773DC1}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4211E5B7-A40C-4F39-A0BD-B28B4E6A2487}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1952,7 +1995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1960,7 +2003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1968,7 +2011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1976,31 +2019,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>